<commit_message>
schema: spreadsheets: Correct spelling of option in spreadsheet
Updates to 3.1.1 of schema
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_v017.xlsx
+++ b/indigo/spreadsheetform_guides/project_v017.xlsx
@@ -3046,12 +3046,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3117,7 +3117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3127,12 +3127,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3173,7 +3172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3183,10 +3182,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,7 +3244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3256,7 +3254,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
@@ -3264,7 +3262,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,7 +3297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>360</v>
       </c>
@@ -3554,7 +3551,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
-      <formula1>"Impact bond design,Financial and commercial modeling,Impact bond investment structure,Capital raise ,Loan arranger,Performance management,Legal counsel,Technical assistance,Other"</formula1>
+      <formula1>"Impact bond design,Financial and commercial modelling,Impact bond investment structure,Capital raise ,Loan arranger,Performance management,Legal counsel,Technical assistance,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3569,7 +3566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3579,9 +3576,8 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.7"/>
@@ -3591,11 +3587,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4343,7 +4337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4353,15 +4347,13 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4828,7 +4820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4838,18 +4830,14 @@
       <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5464,7 +5452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5474,14 +5462,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5975,7 +5960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5985,17 +5970,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6554,7 +6537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6564,10 +6547,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.32"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6857,7 +6839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6867,7 +6849,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
@@ -6880,7 +6862,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7530,7 +7511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7540,14 +7521,12 @@
       <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8178,7 +8157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8188,7 +8167,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
@@ -8196,7 +8175,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9248,7 +9226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9258,10 +9236,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9489,7 +9466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9499,10 +9476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
@@ -9729,7 +9703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9739,11 +9713,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9972,7 +9945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9982,10 +9955,7 @@
       <selection pane="topLeft" activeCell="A249" activeCellId="0" sqref="A249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -11244,7 +11214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -11254,14 +11224,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11454,7 +11423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -11464,7 +11433,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>
@@ -11472,12 +11441,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12096,7 +12063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -12106,7 +12073,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>
@@ -12114,12 +12081,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12714,11 +12679,11 @@
       <formula1>"Purchased or spent,In-kind,Staff cost,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:I32" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A32" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A32" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:I32" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12738,7 +12703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -12748,10 +12713,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12850,7 +12812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -12860,10 +12822,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12952,7 +12911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -12962,7 +12921,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.94"/>
@@ -12973,7 +12932,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13389,7 +13347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13399,7 +13357,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
@@ -13409,10 +13367,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13933,7 +13889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13943,16 +13899,13 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14439,7 +14392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14449,10 +14402,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -14924,7 +14874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14934,7 +14884,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
@@ -14946,7 +14896,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15505,7 +15454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15515,7 +15464,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.9"/>
@@ -15530,7 +15479,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16199,7 +16147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -16209,7 +16157,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
@@ -16218,12 +16166,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
spreadsheets: Fix problem in Project, Investments tab
Excel was reporting an error.

Recreated tab to fix.
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_v017.xlsx
+++ b/indigo/spreadsheetform_guides/project_v017.xlsx
@@ -16,8 +16,8 @@
     <sheet name="Organisations" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Service Provisions" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Outcome Payment Commitments" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Investments" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="InvestmentsOrgRoleOptions" sheetId="10" state="hidden" r:id="rId11"/>
+    <sheet name="InvestmentsOrgRoleOptions" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="Investments" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Intermediary services" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Outcome Metrics" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Outcome Pricing" sheetId="13" state="visible" r:id="rId14"/>
@@ -1009,6 +1009,33 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_payment_commitments:status</t>
   </si>
   <si>
+    <t xml:space="preserve">Nonprofit/NGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundation/Philanthropist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government/Public Sector/Public Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilateral/Bilateral/Intergovernmental Financial Institution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporate Giving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investment Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Net Worth Individual/Family Office/Private Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact Investor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
     <t xml:space="preserve">0-100</t>
   </si>
   <si>
@@ -1042,7 +1069,7 @@
     <t xml:space="preserve">Loss</t>
   </si>
   <si>
-    <t xml:space="preserve">Return 
+    <t xml:space="preserve">Return
 Type</t>
   </si>
   <si>
@@ -1053,7 +1080,8 @@
 Repayment</t>
   </si>
   <si>
-    <t xml:space="preserve">Investment Type</t>
+    <t xml:space="preserve">Investment 
+Type</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:id</t>
@@ -1108,33 +1136,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonprofit/NGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foundation/Philanthropist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government/Public Sector/Public Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilateral/Bilateral/Intergovernmental Financial Institution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corporate Giving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investment Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Net Worth Individual/Family Office/Private Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impact Investor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commercial</t>
   </si>
   <si>
     <t xml:space="preserve">Other Role 
@@ -2809,7 +2810,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2850,6 +2851,22 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2963,7 +2980,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3032,11 +3049,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3127,7 +3164,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.33"/>
@@ -3176,7 +3213,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A2:R40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -3184,55 +3221,893 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="J5" s="20" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="K5" s="20" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="L5" s="20" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="M5" s="20" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="N5" s="20" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="O5" s="20" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="P5" s="21" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="Q5" s="20" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="R5" s="20" t="s">
         <v>358</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="15"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="15"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:R3"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R5:R40" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O40" type="list">
+      <formula1>"Debt,Equity,Combination"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N5:N40" type="list">
+      <formula1>"No repayment (no principle or return),Some repayment (but below value of principle),Principal repaid (but no net return),Principal + positive financial returns,Not publicly available"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:L40" type="list">
+      <formula1>"IRR,Average annual return"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C40" type="list">
+      <formula1>InvestmentsOrgRoleOptions!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3254,7 +4129,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
@@ -3573,10 +4448,10 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
@@ -4344,10 +5219,10 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
@@ -4379,7 +5254,7 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>400</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4827,10 +5702,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.26"/>
@@ -4863,13 +5738,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="22" t="s">
         <v>400</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="22" t="s">
         <v>414</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -5462,7 +6337,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
@@ -5970,7 +6845,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.89"/>
@@ -6008,7 +6883,7 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>452</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -6547,7 +7422,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.32"/>
   </cols>
@@ -6849,7 +7724,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
@@ -6888,7 +7763,7 @@
       <c r="O2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>400</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -7518,10 +8393,10 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
@@ -7539,7 +8414,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="17"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -7552,7 +8427,7 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>400</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -7561,10 +8436,10 @@
       <c r="C3" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="22" t="s">
         <v>549</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="22" t="s">
         <v>550</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -8167,7 +9042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
@@ -9236,7 +10111,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
   </cols>
@@ -9476,7 +10351,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
@@ -9713,7 +10588,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.77"/>
@@ -9955,7 +10830,7 @@
       <selection pane="topLeft" activeCell="A249" activeCellId="0" sqref="A249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -11224,7 +12099,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.26"/>
@@ -11278,7 +12153,7 @@
       <c r="B6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="4"/>
@@ -11433,7 +12308,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>
@@ -12073,7 +12948,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>
@@ -12158,7 +13033,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="24" t="s">
         <v>863</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -12713,7 +13588,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12822,7 +13697,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12921,7 +13796,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.94"/>
@@ -13357,7 +14232,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
@@ -13896,10 +14771,10 @@
   <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
@@ -14402,7 +15277,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -14884,7 +15759,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
@@ -15464,7 +16339,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.9"/>
@@ -16151,771 +17026,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="8"/>
-      <c r="K2" s="0" t="s">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="F4" s="4" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="H4" s="4" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="I4" s="4" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:R3"/>
-  </mergeCells>
-  <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R5:R33" type="list">
-      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
-      <formula2>/</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:L33" type="list">
-      <formula1>"IRR,Average annual return"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N5:N33" type="list">
-      <formula1>"No repayment (no principle or return),Some repayment (but below value of principle),Principal repaid (but no net return),Principal + positive financial returns,Not publicly available"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O33" type="list">
-      <formula1>"Debt,Equity,Combination"</formula1>
-      <formula2>i</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C33" type="list">
-      <formula1>InvestmentsOrgRoleOptions!$A$1:$A$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>